<commit_message>
Adicionado Plano de iteração T2 e atualizado work Items list
</commit_message>
<xml_diff>
--- a/Diretórios/gerentedeprojeto/Work Items List.xlsx
+++ b/Diretórios/gerentedeprojeto/Work Items List.xlsx
@@ -5,23 +5,23 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\15280212\Desktop\wattafood\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\15280212\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="6030"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="51">
   <si>
     <t>Name / Description</t>
   </si>
@@ -135,6 +135,45 @@
   </si>
   <si>
     <t>Mateus</t>
+  </si>
+  <si>
+    <t>Manage Requirements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Find and Outline Requirements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Detail Requirements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Criar Supporting Requirements</t>
+  </si>
+  <si>
+    <t>Revisar/Atualizar Glossário</t>
+  </si>
+  <si>
+    <t>Criar Casos de uso dos requisitos</t>
+  </si>
+  <si>
+    <t>Atualizar o Use-Case Model</t>
+  </si>
+  <si>
+    <t>Atualizar o Working Item List</t>
+  </si>
+  <si>
+    <t>Criar Casos de teste</t>
+  </si>
+  <si>
+    <t>Atualizar architecture handbook</t>
+  </si>
+  <si>
+    <t>Criar Documento de Desigin</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lucilene</t>
+  </si>
+  <si>
+    <t>Implementar Teste (Descrever detalhadamente os casos de teste)</t>
   </si>
 </sst>
 </file>
@@ -254,7 +293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -332,6 +371,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -612,10 +652,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1005"/>
+  <dimension ref="A1:Z1018"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -955,285 +995,426 @@
       <c r="I13" s="14"/>
     </row>
     <row r="14" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A14" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="18"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="34"/>
+      <c r="A14" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="28"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="13"/>
       <c r="I14" s="14"/>
     </row>
     <row r="15" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A15" s="25" t="s">
-        <v>23</v>
+      <c r="A15" s="14" t="s">
+        <v>39</v>
       </c>
       <c r="B15" s="28">
         <v>1</v>
       </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="24" t="s">
+      <c r="C15" s="18"/>
+      <c r="D15" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="4"/>
-      <c r="F15" s="12"/>
+      <c r="E15" s="7">
+        <v>2</v>
+      </c>
+      <c r="F15" s="35" t="s">
+        <v>33</v>
+      </c>
       <c r="G15" s="11"/>
       <c r="H15" s="13"/>
       <c r="I15" s="14"/>
     </row>
     <row r="16" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A16" s="25" t="s">
-        <v>24</v>
+      <c r="A16" s="14" t="s">
+        <v>41</v>
       </c>
       <c r="B16" s="28">
-        <v>1</v>
-      </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="18"/>
+      <c r="D16" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="12"/>
+      <c r="E16" s="7">
+        <v>2</v>
+      </c>
+      <c r="F16" s="35" t="s">
+        <v>33</v>
+      </c>
       <c r="G16" s="11"/>
       <c r="H16" s="13"/>
       <c r="I16" s="14"/>
     </row>
     <row r="17" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A17" s="25" t="s">
-        <v>25</v>
+      <c r="A17" s="14" t="s">
+        <v>40</v>
       </c>
       <c r="B17" s="28">
         <v>2</v>
       </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="24" t="s">
+      <c r="C17" s="18"/>
+      <c r="D17" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E17" s="4"/>
-      <c r="F17" s="12"/>
+      <c r="E17" s="7">
+        <v>2</v>
+      </c>
+      <c r="F17" s="35" t="s">
+        <v>33</v>
+      </c>
       <c r="G17" s="11"/>
       <c r="H17" s="13"/>
       <c r="I17" s="14"/>
     </row>
     <row r="18" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A18" s="25" t="s">
-        <v>26</v>
+      <c r="A18" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="B18" s="28">
         <v>4</v>
       </c>
-      <c r="C18" s="10"/>
-      <c r="D18" s="24" t="s">
+      <c r="C18" s="18"/>
+      <c r="D18" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E18" s="4"/>
-      <c r="F18" s="12"/>
+      <c r="E18" s="7">
+        <v>2</v>
+      </c>
+      <c r="F18" s="35" t="s">
+        <v>34</v>
+      </c>
       <c r="G18" s="11"/>
       <c r="H18" s="13"/>
       <c r="I18" s="14"/>
     </row>
     <row r="19" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A19" s="25" t="s">
-        <v>27</v>
+      <c r="A19" s="14" t="s">
+        <v>43</v>
       </c>
       <c r="B19" s="28">
-        <v>4</v>
-      </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="18"/>
+      <c r="D19" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="4"/>
-      <c r="F19" s="12"/>
+      <c r="E19" s="7">
+        <v>2</v>
+      </c>
+      <c r="F19" s="35" t="s">
+        <v>33</v>
+      </c>
       <c r="G19" s="11"/>
       <c r="H19" s="13"/>
       <c r="I19" s="14"/>
     </row>
     <row r="20" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A20" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="B20" s="18">
+      <c r="A20" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="28">
         <v>3</v>
       </c>
-      <c r="C20" s="15"/>
-      <c r="D20" s="32" t="s">
+      <c r="C20" s="18"/>
+      <c r="D20" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E20" s="4"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="14"/>
+      <c r="E20" s="7">
+        <v>2</v>
+      </c>
+      <c r="F20" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="G20" s="11"/>
+      <c r="H20" s="13"/>
       <c r="I20" s="14"/>
     </row>
     <row r="21" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A21" s="25" t="s">
-        <v>29</v>
+      <c r="A21" s="14" t="s">
+        <v>45</v>
       </c>
       <c r="B21" s="28">
-        <v>4</v>
-      </c>
-      <c r="C21" s="10"/>
-      <c r="D21" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="18"/>
+      <c r="D21" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E21" s="18"/>
-      <c r="F21" s="12"/>
+      <c r="E21" s="7">
+        <v>2</v>
+      </c>
+      <c r="F21" s="35" t="s">
+        <v>34</v>
+      </c>
       <c r="G21" s="11"/>
       <c r="H21" s="13"/>
       <c r="I21" s="14"/>
     </row>
     <row r="22" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A22" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22" s="18">
+      <c r="A22" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="28">
+        <v>1</v>
+      </c>
+      <c r="C22" s="18"/>
+      <c r="D22" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="7">
+        <v>2</v>
+      </c>
+      <c r="F22" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="G22" s="11"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="14"/>
+    </row>
+    <row r="23" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A23" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" s="28">
+        <v>1</v>
+      </c>
+      <c r="C23" s="18"/>
+      <c r="D23" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="7">
+        <v>2</v>
+      </c>
+      <c r="F23" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="G23" s="11"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="14"/>
+    </row>
+    <row r="24" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A24" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" s="28">
+        <v>2</v>
+      </c>
+      <c r="C24" s="18"/>
+      <c r="D24" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="7">
+        <v>2</v>
+      </c>
+      <c r="F24" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="G24" s="11"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="14"/>
+    </row>
+    <row r="25" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A25" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" s="29">
+        <v>2</v>
+      </c>
+      <c r="C25" s="18"/>
+      <c r="D25" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="7">
+        <v>2</v>
+      </c>
+      <c r="F25" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="G25" s="11"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="14"/>
+    </row>
+    <row r="26" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A26" s="25"/>
+      <c r="B26" s="28"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="33"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="14"/>
+    </row>
+    <row r="27" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A27" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="18"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="34"/>
+      <c r="I27" s="14"/>
+    </row>
+    <row r="28" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A28" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="28">
+        <v>1</v>
+      </c>
+      <c r="C28" s="10"/>
+      <c r="D28" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="4"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="14"/>
+    </row>
+    <row r="29" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A29" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" s="28">
+        <v>1</v>
+      </c>
+      <c r="C29" s="10"/>
+      <c r="D29" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="4"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="14"/>
+    </row>
+    <row r="30" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A30" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" s="28">
+        <v>2</v>
+      </c>
+      <c r="C30" s="10"/>
+      <c r="D30" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="4"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="14"/>
+    </row>
+    <row r="31" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A31" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" s="28">
         <v>4</v>
       </c>
-      <c r="C22" s="15"/>
-      <c r="D22" s="25" t="s">
+      <c r="C31" s="10"/>
+      <c r="D31" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="F22" s="16"/>
-      <c r="G22" s="14"/>
-      <c r="I22" s="14"/>
-    </row>
-    <row r="23" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A23" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23" s="28">
+      <c r="E31" s="4"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="14"/>
+    </row>
+    <row r="32" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A32" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32" s="28">
         <v>4</v>
       </c>
-      <c r="C23" s="10"/>
-      <c r="D23" s="26" t="s">
+      <c r="C32" s="10"/>
+      <c r="D32" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="F23" s="12"/>
-      <c r="G23" s="14"/>
-      <c r="I23" s="14"/>
-    </row>
-    <row r="24" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A24" s="11"/>
-      <c r="B24" s="28"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="I24" s="14"/>
-    </row>
-    <row r="25" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A25" s="11"/>
-      <c r="B25" s="28"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="11"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="14"/>
-      <c r="I25" s="14"/>
-    </row>
-    <row r="26" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A26" s="11"/>
-      <c r="B26" s="28"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="11"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="14"/>
-      <c r="I26" s="14"/>
-    </row>
-    <row r="27" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A27" s="11"/>
-      <c r="B27" s="28"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="11"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="14"/>
-      <c r="I27" s="14"/>
-    </row>
-    <row r="28" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A28" s="11"/>
-      <c r="B28" s="28"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="11"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="14"/>
-      <c r="I28" s="14"/>
-    </row>
-    <row r="29" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A29" s="11"/>
-      <c r="B29" s="28"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="14"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="14"/>
-      <c r="I29" s="14"/>
-    </row>
-    <row r="30" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A30" s="11"/>
-      <c r="B30" s="28"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="11"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="14"/>
-      <c r="I30" s="14"/>
-    </row>
-    <row r="31" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A31" s="11"/>
-      <c r="B31" s="28"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="11"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="14"/>
-      <c r="I31" s="14"/>
-    </row>
-    <row r="32" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A32" s="11"/>
-      <c r="B32" s="28"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="11"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="14"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="13"/>
       <c r="I32" s="14"/>
     </row>
     <row r="33" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A33" s="11"/>
-      <c r="B33" s="28"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="11"/>
-      <c r="F33" s="19"/>
+      <c r="A33" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B33" s="18">
+        <v>3</v>
+      </c>
+      <c r="C33" s="15"/>
+      <c r="D33" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="4"/>
+      <c r="F33" s="16"/>
       <c r="G33" s="14"/>
       <c r="I33" s="14"/>
     </row>
     <row r="34" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A34" s="13"/>
-      <c r="B34" s="30"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="13"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="14"/>
+      <c r="A34" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34" s="28">
+        <v>4</v>
+      </c>
+      <c r="C34" s="10"/>
+      <c r="D34" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" s="18"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="13"/>
       <c r="I34" s="14"/>
     </row>
     <row r="35" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A35" s="13"/>
-      <c r="B35" s="30"/>
-      <c r="C35" s="20"/>
-      <c r="D35" s="13"/>
+      <c r="A35" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B35" s="18">
+        <v>4</v>
+      </c>
+      <c r="C35" s="15"/>
+      <c r="D35" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="F35" s="16"/>
       <c r="G35" s="14"/>
       <c r="I35" s="14"/>
     </row>
     <row r="36" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A36" s="11"/>
-      <c r="B36" s="28"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="14"/>
+      <c r="A36" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="B36" s="28">
+        <v>4</v>
+      </c>
+      <c r="C36" s="10"/>
+      <c r="D36" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="F36" s="12"/>
       <c r="G36" s="14"/>
       <c r="I36" s="14"/>
     </row>
     <row r="37" spans="1:9" ht="12.75" customHeight="1">
       <c r="A37" s="11"/>
-      <c r="B37" s="30"/>
-      <c r="C37" s="20"/>
-      <c r="D37" s="13"/>
+      <c r="B37" s="28"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="14"/>
       <c r="G37" s="14"/>
       <c r="I37" s="14"/>
     </row>
@@ -1241,38 +1422,44 @@
       <c r="A38" s="11"/>
       <c r="B38" s="28"/>
       <c r="C38" s="10"/>
-      <c r="D38" s="13"/>
+      <c r="D38" s="11"/>
+      <c r="F38" s="19"/>
       <c r="G38" s="14"/>
       <c r="I38" s="14"/>
     </row>
     <row r="39" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A39" s="13"/>
-      <c r="B39" s="30"/>
-      <c r="C39" s="20"/>
-      <c r="D39" s="13"/>
+      <c r="A39" s="11"/>
+      <c r="B39" s="28"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="11"/>
+      <c r="F39" s="19"/>
       <c r="G39" s="14"/>
       <c r="I39" s="14"/>
     </row>
     <row r="40" spans="1:9" ht="12.75" customHeight="1">
       <c r="A40" s="11"/>
-      <c r="B40" s="30"/>
-      <c r="C40" s="20"/>
-      <c r="D40" s="13"/>
+      <c r="B40" s="28"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="11"/>
+      <c r="F40" s="19"/>
       <c r="G40" s="14"/>
       <c r="I40" s="14"/>
     </row>
     <row r="41" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A41" s="13"/>
-      <c r="B41" s="30"/>
-      <c r="C41" s="21"/>
+      <c r="A41" s="11"/>
+      <c r="B41" s="28"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="11"/>
+      <c r="F41" s="19"/>
       <c r="G41" s="14"/>
       <c r="I41" s="14"/>
     </row>
     <row r="42" spans="1:9" ht="12.75" customHeight="1">
       <c r="A42" s="11"/>
       <c r="B42" s="28"/>
-      <c r="C42" s="10"/>
-      <c r="D42" s="11"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="14"/>
+      <c r="F42" s="19"/>
       <c r="G42" s="14"/>
       <c r="I42" s="14"/>
     </row>
@@ -1280,7 +1467,8 @@
       <c r="A43" s="11"/>
       <c r="B43" s="28"/>
       <c r="C43" s="10"/>
-      <c r="D43" s="13"/>
+      <c r="D43" s="11"/>
+      <c r="F43" s="19"/>
       <c r="G43" s="14"/>
       <c r="I43" s="14"/>
     </row>
@@ -1289,37 +1477,41 @@
       <c r="B44" s="28"/>
       <c r="C44" s="10"/>
       <c r="D44" s="11"/>
+      <c r="F44" s="19"/>
       <c r="G44" s="14"/>
       <c r="I44" s="14"/>
     </row>
     <row r="45" spans="1:9" ht="12.75" customHeight="1">
       <c r="A45" s="11"/>
       <c r="B45" s="28"/>
-      <c r="C45" s="15"/>
-      <c r="D45" s="14"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="11"/>
+      <c r="F45" s="19"/>
       <c r="G45" s="14"/>
       <c r="I45" s="14"/>
     </row>
     <row r="46" spans="1:9" ht="12.75" customHeight="1">
       <c r="A46" s="11"/>
-      <c r="B46" s="30"/>
+      <c r="B46" s="28"/>
       <c r="C46" s="10"/>
-      <c r="D46" s="13"/>
+      <c r="D46" s="11"/>
+      <c r="F46" s="19"/>
       <c r="G46" s="14"/>
       <c r="I46" s="14"/>
     </row>
     <row r="47" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A47" s="11"/>
-      <c r="B47" s="28"/>
-      <c r="C47" s="10"/>
+      <c r="A47" s="13"/>
+      <c r="B47" s="30"/>
+      <c r="C47" s="20"/>
       <c r="D47" s="13"/>
+      <c r="F47" s="19"/>
       <c r="G47" s="14"/>
       <c r="I47" s="14"/>
     </row>
     <row r="48" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A48" s="11"/>
-      <c r="B48" s="28"/>
-      <c r="C48" s="10"/>
+      <c r="A48" s="13"/>
+      <c r="B48" s="30"/>
+      <c r="C48" s="20"/>
       <c r="D48" s="13"/>
       <c r="G48" s="14"/>
       <c r="I48" s="14"/>
@@ -1327,15 +1519,15 @@
     <row r="49" spans="1:9" ht="12.75" customHeight="1">
       <c r="A49" s="11"/>
       <c r="B49" s="28"/>
-      <c r="C49" s="10"/>
-      <c r="D49" s="13"/>
+      <c r="C49" s="15"/>
+      <c r="D49" s="14"/>
       <c r="G49" s="14"/>
       <c r="I49" s="14"/>
     </row>
     <row r="50" spans="1:9" ht="12.75" customHeight="1">
       <c r="A50" s="11"/>
-      <c r="B50" s="28"/>
-      <c r="C50" s="10"/>
+      <c r="B50" s="30"/>
+      <c r="C50" s="20"/>
       <c r="D50" s="13"/>
       <c r="G50" s="14"/>
       <c r="I50" s="14"/>
@@ -1349,114 +1541,113 @@
       <c r="I51" s="14"/>
     </row>
     <row r="52" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A52" s="11"/>
-      <c r="B52" s="28"/>
-      <c r="C52" s="10"/>
+      <c r="A52" s="13"/>
+      <c r="B52" s="30"/>
+      <c r="C52" s="20"/>
       <c r="D52" s="13"/>
       <c r="G52" s="14"/>
       <c r="I52" s="14"/>
     </row>
     <row r="53" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A53" s="14"/>
-      <c r="B53" s="18"/>
-      <c r="C53" s="14"/>
-      <c r="D53" s="14"/>
+      <c r="A53" s="11"/>
+      <c r="B53" s="30"/>
+      <c r="C53" s="20"/>
+      <c r="D53" s="13"/>
       <c r="G53" s="14"/>
       <c r="I53" s="14"/>
     </row>
     <row r="54" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A54" s="14"/>
-      <c r="B54" s="18"/>
-      <c r="C54" s="14"/>
-      <c r="D54" s="14"/>
+      <c r="A54" s="13"/>
+      <c r="B54" s="30"/>
+      <c r="C54" s="21"/>
       <c r="G54" s="14"/>
       <c r="I54" s="14"/>
     </row>
     <row r="55" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A55" s="14"/>
-      <c r="B55" s="18"/>
-      <c r="C55" s="14"/>
-      <c r="D55" s="14"/>
+      <c r="A55" s="11"/>
+      <c r="B55" s="28"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="11"/>
       <c r="G55" s="14"/>
       <c r="I55" s="14"/>
     </row>
     <row r="56" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A56" s="14"/>
-      <c r="B56" s="18"/>
-      <c r="C56" s="14"/>
-      <c r="D56" s="14"/>
+      <c r="A56" s="11"/>
+      <c r="B56" s="28"/>
+      <c r="C56" s="10"/>
+      <c r="D56" s="13"/>
       <c r="G56" s="14"/>
       <c r="I56" s="14"/>
     </row>
     <row r="57" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A57" s="14"/>
-      <c r="B57" s="18"/>
-      <c r="C57" s="14"/>
-      <c r="D57" s="14"/>
+      <c r="A57" s="11"/>
+      <c r="B57" s="28"/>
+      <c r="C57" s="10"/>
+      <c r="D57" s="11"/>
       <c r="G57" s="14"/>
       <c r="I57" s="14"/>
     </row>
     <row r="58" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A58" s="14"/>
-      <c r="B58" s="18"/>
-      <c r="C58" s="11"/>
+      <c r="A58" s="11"/>
+      <c r="B58" s="28"/>
+      <c r="C58" s="15"/>
       <c r="D58" s="14"/>
       <c r="G58" s="14"/>
       <c r="I58" s="14"/>
     </row>
     <row r="59" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A59" s="14"/>
-      <c r="B59" s="18"/>
-      <c r="C59" s="14"/>
-      <c r="D59" s="14"/>
+      <c r="A59" s="11"/>
+      <c r="B59" s="30"/>
+      <c r="C59" s="10"/>
+      <c r="D59" s="13"/>
       <c r="G59" s="14"/>
       <c r="I59" s="14"/>
     </row>
     <row r="60" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A60" s="14"/>
-      <c r="B60" s="18"/>
-      <c r="C60" s="11"/>
-      <c r="D60" s="14"/>
+      <c r="A60" s="11"/>
+      <c r="B60" s="28"/>
+      <c r="C60" s="10"/>
+      <c r="D60" s="13"/>
       <c r="G60" s="14"/>
       <c r="I60" s="14"/>
     </row>
     <row r="61" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A61" s="14"/>
-      <c r="B61" s="18"/>
-      <c r="C61" s="11"/>
-      <c r="D61" s="14"/>
+      <c r="A61" s="11"/>
+      <c r="B61" s="28"/>
+      <c r="C61" s="10"/>
+      <c r="D61" s="13"/>
       <c r="G61" s="14"/>
       <c r="I61" s="14"/>
     </row>
     <row r="62" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A62" s="14"/>
-      <c r="B62" s="18"/>
-      <c r="C62" s="14"/>
-      <c r="D62" s="14"/>
+      <c r="A62" s="11"/>
+      <c r="B62" s="28"/>
+      <c r="C62" s="10"/>
+      <c r="D62" s="13"/>
       <c r="G62" s="14"/>
       <c r="I62" s="14"/>
     </row>
     <row r="63" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A63" s="14"/>
-      <c r="B63" s="18"/>
-      <c r="C63" s="14"/>
-      <c r="D63" s="14"/>
+      <c r="A63" s="11"/>
+      <c r="B63" s="28"/>
+      <c r="C63" s="10"/>
+      <c r="D63" s="13"/>
       <c r="G63" s="14"/>
       <c r="I63" s="14"/>
     </row>
     <row r="64" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A64" s="14"/>
-      <c r="B64" s="18"/>
-      <c r="C64" s="14"/>
-      <c r="D64" s="14"/>
+      <c r="A64" s="11"/>
+      <c r="B64" s="28"/>
+      <c r="C64" s="10"/>
+      <c r="D64" s="13"/>
       <c r="G64" s="14"/>
       <c r="I64" s="14"/>
     </row>
     <row r="65" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A65" s="14"/>
-      <c r="B65" s="18"/>
-      <c r="C65" s="14"/>
-      <c r="D65" s="14"/>
+      <c r="A65" s="11"/>
+      <c r="B65" s="28"/>
+      <c r="C65" s="10"/>
+      <c r="D65" s="13"/>
       <c r="G65" s="14"/>
       <c r="I65" s="14"/>
     </row>
@@ -1503,7 +1694,7 @@
     <row r="71" spans="1:9" ht="12.75" customHeight="1">
       <c r="A71" s="14"/>
       <c r="B71" s="18"/>
-      <c r="C71" s="14"/>
+      <c r="C71" s="11"/>
       <c r="D71" s="14"/>
       <c r="G71" s="14"/>
       <c r="I71" s="14"/>
@@ -1519,7 +1710,7 @@
     <row r="73" spans="1:9" ht="12.75" customHeight="1">
       <c r="A73" s="14"/>
       <c r="B73" s="18"/>
-      <c r="C73" s="14"/>
+      <c r="C73" s="11"/>
       <c r="D73" s="14"/>
       <c r="G73" s="14"/>
       <c r="I73" s="14"/>
@@ -1527,7 +1718,7 @@
     <row r="74" spans="1:9" ht="12.75" customHeight="1">
       <c r="A74" s="14"/>
       <c r="B74" s="18"/>
-      <c r="C74" s="14"/>
+      <c r="C74" s="11"/>
       <c r="D74" s="14"/>
       <c r="G74" s="14"/>
       <c r="I74" s="14"/>
@@ -8979,6 +9170,110 @@
       <c r="D1005" s="14"/>
       <c r="G1005" s="14"/>
       <c r="I1005" s="14"/>
+    </row>
+    <row r="1006" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A1006" s="14"/>
+      <c r="B1006" s="18"/>
+      <c r="C1006" s="14"/>
+      <c r="D1006" s="14"/>
+      <c r="G1006" s="14"/>
+      <c r="I1006" s="14"/>
+    </row>
+    <row r="1007" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A1007" s="14"/>
+      <c r="B1007" s="18"/>
+      <c r="C1007" s="14"/>
+      <c r="D1007" s="14"/>
+      <c r="G1007" s="14"/>
+      <c r="I1007" s="14"/>
+    </row>
+    <row r="1008" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A1008" s="14"/>
+      <c r="B1008" s="18"/>
+      <c r="C1008" s="14"/>
+      <c r="D1008" s="14"/>
+      <c r="G1008" s="14"/>
+      <c r="I1008" s="14"/>
+    </row>
+    <row r="1009" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A1009" s="14"/>
+      <c r="B1009" s="18"/>
+      <c r="C1009" s="14"/>
+      <c r="D1009" s="14"/>
+      <c r="G1009" s="14"/>
+      <c r="I1009" s="14"/>
+    </row>
+    <row r="1010" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A1010" s="14"/>
+      <c r="B1010" s="18"/>
+      <c r="C1010" s="14"/>
+      <c r="D1010" s="14"/>
+      <c r="G1010" s="14"/>
+      <c r="I1010" s="14"/>
+    </row>
+    <row r="1011" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A1011" s="14"/>
+      <c r="B1011" s="18"/>
+      <c r="C1011" s="14"/>
+      <c r="D1011" s="14"/>
+      <c r="G1011" s="14"/>
+      <c r="I1011" s="14"/>
+    </row>
+    <row r="1012" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A1012" s="14"/>
+      <c r="B1012" s="18"/>
+      <c r="C1012" s="14"/>
+      <c r="D1012" s="14"/>
+      <c r="G1012" s="14"/>
+      <c r="I1012" s="14"/>
+    </row>
+    <row r="1013" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A1013" s="14"/>
+      <c r="B1013" s="18"/>
+      <c r="C1013" s="14"/>
+      <c r="D1013" s="14"/>
+      <c r="G1013" s="14"/>
+      <c r="I1013" s="14"/>
+    </row>
+    <row r="1014" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A1014" s="14"/>
+      <c r="B1014" s="18"/>
+      <c r="C1014" s="14"/>
+      <c r="D1014" s="14"/>
+      <c r="G1014" s="14"/>
+      <c r="I1014" s="14"/>
+    </row>
+    <row r="1015" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A1015" s="14"/>
+      <c r="B1015" s="18"/>
+      <c r="C1015" s="14"/>
+      <c r="D1015" s="14"/>
+      <c r="G1015" s="14"/>
+      <c r="I1015" s="14"/>
+    </row>
+    <row r="1016" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A1016" s="14"/>
+      <c r="B1016" s="18"/>
+      <c r="C1016" s="14"/>
+      <c r="D1016" s="14"/>
+      <c r="G1016" s="14"/>
+      <c r="I1016" s="14"/>
+    </row>
+    <row r="1017" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A1017" s="14"/>
+      <c r="B1017" s="18"/>
+      <c r="C1017" s="14"/>
+      <c r="D1017" s="14"/>
+      <c r="G1017" s="14"/>
+      <c r="I1017" s="14"/>
+    </row>
+    <row r="1018" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A1018" s="14"/>
+      <c r="B1018" s="18"/>
+      <c r="C1018" s="14"/>
+      <c r="D1018" s="14"/>
+      <c r="G1018" s="14"/>
+      <c r="I1018" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>